<commit_message>
severe by age scsv synced
</commit_message>
<xml_diff>
--- a/data/Israel/infected_abroad.xlsx
+++ b/data/Israel/infected_abroad.xlsx
@@ -148,15 +148,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A116" activeCellId="0" sqref="A116:A117"/>
+      <selection pane="bottomLeft" activeCell="E116" activeCellId="0" sqref="E116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
     <col min="2" max="2" width="7.7109375" style="0" hidden="false" customWidth="true" outlineLevel="0" collapsed="false"/>
@@ -311,7 +311,7 @@
         <v>44300</v>
       </c>
       <c r="B9">
-        <v>51475</v>
+        <v>51476</v>
       </c>
       <c r="C9">
         <v>202</v>
@@ -624,10 +624,10 @@
         <v>44317</v>
       </c>
       <c r="B26">
-        <v>9135</v>
+        <v>9169</v>
       </c>
       <c r="C26">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -1684,7 +1684,7 @@
         <v>44376</v>
       </c>
       <c r="B85">
-        <v>46863</v>
+        <v>46864</v>
       </c>
       <c r="C85">
         <v>294</v>
@@ -2058,7 +2058,7 @@
         <v>44398</v>
       </c>
       <c r="B107">
-        <v>85830</v>
+        <v>85831</v>
       </c>
       <c r="C107">
         <v>1350</v>
@@ -2095,7 +2095,7 @@
         <v>98197</v>
       </c>
       <c r="C109">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="D109">
         <v>1301</v>
@@ -2146,7 +2146,7 @@
         <v>102846</v>
       </c>
       <c r="C112">
-        <v>2143</v>
+        <v>2144</v>
       </c>
       <c r="D112">
         <v>1944</v>
@@ -2160,10 +2160,10 @@
         <v>44404</v>
       </c>
       <c r="B113">
-        <v>106070</v>
+        <v>106072</v>
       </c>
       <c r="C113">
-        <v>2298</v>
+        <v>2300</v>
       </c>
       <c r="D113">
         <v>2102</v>
@@ -2177,10 +2177,10 @@
         <v>44405</v>
       </c>
       <c r="B114">
-        <v>102771</v>
+        <v>102790</v>
       </c>
       <c r="C114">
-        <v>2197</v>
+        <v>2200</v>
       </c>
       <c r="D114">
         <v>2066</v>
@@ -2194,16 +2194,16 @@
         <v>44406</v>
       </c>
       <c r="B115">
-        <v>101791</v>
+        <v>101793</v>
       </c>
       <c r="C115">
-        <v>2176</v>
+        <v>2183</v>
       </c>
       <c r="D115">
-        <v>1998</v>
+        <v>2005</v>
       </c>
       <c r="E115">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,13 +2211,13 @@
         <v>44407</v>
       </c>
       <c r="B116">
-        <v>111064</v>
+        <v>111114</v>
       </c>
       <c r="C116">
-        <v>2459</v>
+        <v>2460</v>
       </c>
       <c r="D116">
-        <v>2237</v>
+        <v>2238</v>
       </c>
       <c r="E116">
         <v>221</v>
@@ -2228,16 +2228,33 @@
         <v>44408</v>
       </c>
       <c r="B117">
-        <v>73710</v>
+        <v>73892</v>
       </c>
       <c r="C117">
-        <v>2108</v>
+        <v>2117</v>
       </c>
       <c r="D117">
-        <v>1914</v>
+        <v>1929</v>
       </c>
       <c r="E117">
         <v>194</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="5">
+        <v>44409</v>
+      </c>
+      <c r="B118">
+        <v>80647</v>
+      </c>
+      <c r="C118">
+        <v>2132</v>
+      </c>
+      <c r="D118">
+        <v>1932</v>
+      </c>
+      <c r="E118">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>